<commit_message>
Instructor Automation testing Added
</commit_message>
<xml_diff>
--- a/Test Cases and Reports/Manual Testing Reports/Test Case Report.xlsx
+++ b/Test Cases and Reports/Manual Testing Reports/Test Case Report.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sheme\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sheme\Downloads\Voice-Enabled-AI-Chatbot\Test Cases and Reports\Manual Testing Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FA27F58-84C8-40E1-88D4-D7E0F17995A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71C23C1D-6B46-4884-AE00-20C26E7AB8B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="7" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Welcome Page" sheetId="1" r:id="rId1"/>
@@ -6522,8 +6522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45843788-D55B-474A-9CF9-D1E9A71CB1B5}">
   <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:J1048576"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -8170,7 +8170,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03BFE7D4-6EFD-421D-98A4-4182420FBABA}">
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -8237,7 +8237,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="96.6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>910</v>
       </c>
@@ -8281,7 +8281,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="69" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>913</v>
       </c>
@@ -8325,7 +8325,7 @@
         <v>918</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="82.8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>946</v>
       </c>
@@ -8369,7 +8369,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="82.8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>946</v>
       </c>
@@ -8413,7 +8413,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="69" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>947</v>
       </c>
@@ -8457,7 +8457,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="69" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>947</v>
       </c>
@@ -8501,7 +8501,7 @@
         <v>962</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="69" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>925</v>
       </c>
@@ -8545,7 +8545,7 @@
         <v>928</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="69" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>925</v>
       </c>
@@ -8589,7 +8589,7 @@
         <v>959</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="69" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>929</v>
       </c>
@@ -8633,7 +8633,7 @@
         <v>932</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="69" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>929</v>
       </c>
@@ -8677,7 +8677,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="69" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>933</v>
       </c>
@@ -8721,7 +8721,7 @@
         <v>936</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="82.8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>937</v>
       </c>
@@ -8765,7 +8765,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="82.8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>937</v>
       </c>
@@ -8809,7 +8809,7 @@
         <v>952</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="69" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>940</v>
       </c>
@@ -8853,7 +8853,7 @@
         <v>941</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="82.8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>942</v>
       </c>
@@ -8897,7 +8897,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="82.8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>942</v>
       </c>
@@ -9192,7 +9192,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="69" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>98</v>
       </c>
@@ -9236,7 +9236,7 @@
         <v>892</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="110.4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>95</v>
       </c>
@@ -9280,7 +9280,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="69" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>92</v>
       </c>
@@ -9324,7 +9324,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="82.8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>89</v>
       </c>
@@ -9368,7 +9368,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="82.8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>89</v>
       </c>
@@ -9412,7 +9412,7 @@
         <v>880</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="124.2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>877</v>
       </c>
@@ -9456,7 +9456,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="124.2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>877</v>
       </c>
@@ -9500,7 +9500,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="82.8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>227</v>
       </c>
@@ -9544,7 +9544,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="110.4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>229</v>
       </c>

</xml_diff>

<commit_message>
Test Case Reports Added
</commit_message>
<xml_diff>
--- a/Test Cases and Reports/Manual Testing Reports/Test Case Report.xlsx
+++ b/Test Cases and Reports/Manual Testing Reports/Test Case Report.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sheme\Downloads\Voice-Enabled-AI-Chatbot\Test Cases and Reports\Manual Testing Reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sheme\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71C23C1D-6B46-4884-AE00-20C26E7AB8B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FA27F58-84C8-40E1-88D4-D7E0F17995A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="7" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Welcome Page" sheetId="1" r:id="rId1"/>
@@ -6522,8 +6522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45843788-D55B-474A-9CF9-D1E9A71CB1B5}">
   <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -8170,7 +8170,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03BFE7D4-6EFD-421D-98A4-4182420FBABA}">
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -8237,7 +8237,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="96.6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>910</v>
       </c>
@@ -8281,7 +8281,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="69" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>913</v>
       </c>
@@ -8325,7 +8325,7 @@
         <v>918</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="82.8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>946</v>
       </c>
@@ -8369,7 +8369,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="82.8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>946</v>
       </c>
@@ -8413,7 +8413,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="69" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>947</v>
       </c>
@@ -8457,7 +8457,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="69" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>947</v>
       </c>
@@ -8501,7 +8501,7 @@
         <v>962</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="69" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>925</v>
       </c>
@@ -8545,7 +8545,7 @@
         <v>928</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="69" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>925</v>
       </c>
@@ -8589,7 +8589,7 @@
         <v>959</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="69" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>929</v>
       </c>
@@ -8633,7 +8633,7 @@
         <v>932</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="69" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>929</v>
       </c>
@@ -8677,7 +8677,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="69" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>933</v>
       </c>
@@ -8721,7 +8721,7 @@
         <v>936</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="82.8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>937</v>
       </c>
@@ -8765,7 +8765,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="82.8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>937</v>
       </c>
@@ -8809,7 +8809,7 @@
         <v>952</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="69" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>940</v>
       </c>
@@ -8853,7 +8853,7 @@
         <v>941</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" ht="82.8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>942</v>
       </c>
@@ -8897,7 +8897,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" ht="82.8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>942</v>
       </c>
@@ -9192,7 +9192,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="69" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>98</v>
       </c>
@@ -9236,7 +9236,7 @@
         <v>892</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="110.4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>95</v>
       </c>
@@ -9280,7 +9280,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="69" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>92</v>
       </c>
@@ -9324,7 +9324,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="82.8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>89</v>
       </c>
@@ -9368,7 +9368,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="82.8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>89</v>
       </c>
@@ -9412,7 +9412,7 @@
         <v>880</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="124.2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>877</v>
       </c>
@@ -9456,7 +9456,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="124.2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>877</v>
       </c>
@@ -9500,7 +9500,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="82.8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>227</v>
       </c>
@@ -9544,7 +9544,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="110.4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>229</v>
       </c>

</xml_diff>